<commit_message>
minor changes in naming
</commit_message>
<xml_diff>
--- a/Chapter 6 Input & Output/monthly_expenses.xlsx
+++ b/Chapter 6 Input & Output/monthly_expenses.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
@@ -487,6 +487,16 @@
           <t>Savings Oppurtunity</t>
         </is>
       </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Expenses type</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Saving opportunity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -517,6 +527,16 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -547,6 +567,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -577,6 +607,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -607,6 +647,16 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -637,6 +687,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -667,6 +727,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -697,6 +767,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -727,6 +807,16 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -757,6 +847,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -787,6 +887,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -817,6 +927,16 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -847,6 +967,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -877,6 +1007,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -907,6 +1047,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -937,6 +1087,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -967,6 +1127,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -997,6 +1167,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1027,6 +1207,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1057,6 +1247,16 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1083,6 +1283,16 @@
         </is>
       </c>
       <c r="F21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>